<commit_message>
Removed /test-output/ folder from staged changes
</commit_message>
<xml_diff>
--- a/src/main/java/resources/domainsList.xlsx
+++ b/src/main/java/resources/domainsList.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>List</t>
   </si>
@@ -45,37 +45,7 @@
     <t>https://qualityhirings.com/job/hooters-of-america/indiana-sellersburg-hooter-girl-6cyibxgh9231</t>
   </si>
   <si>
-    <t>employglow.com</t>
-  </si>
-  <si>
-    <t>projobstoday.com</t>
-  </si>
-  <si>
-    <t>hirecurrently.com</t>
-  </si>
-  <si>
-    <t>proworkemploy.com</t>
-  </si>
-  <si>
-    <t>talent-workforce.com</t>
-  </si>
-  <si>
-    <t>jobzcurrently.com</t>
-  </si>
-  <si>
-    <t>topratedjobz.com</t>
-  </si>
-  <si>
-    <t>nurseslistings.com</t>
-  </si>
-  <si>
-    <t>healthcare-listings.com</t>
-  </si>
-  <si>
-    <t>recruitmedix.com</t>
-  </si>
-  <si>
-    <t>seekerhirings.com</t>
+    <t>https://nursesopenings.com/</t>
   </si>
 </sst>
 </file>
@@ -107,27 +77,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -137,7 +92,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -419,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -440,59 +395,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>